<commit_message>
another attempt at replacing local version of spectroscopy branch
</commit_message>
<xml_diff>
--- a/lib/korek/korek_data.xlsx
+++ b/lib/korek/korek_data.xlsx
@@ -13,7 +13,331 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>X1S</t>
+  </si>
+  <si>
+    <t>a3S</t>
+  </si>
+  <si>
+    <t>b3P</t>
+  </si>
+  <si>
+    <t>A1S</t>
+  </si>
+  <si>
+    <t>c3S</t>
+  </si>
+  <si>
+    <t>B1P</t>
+  </si>
+  <si>
+    <t>d3P</t>
+  </si>
+  <si>
+    <t>C1S</t>
+  </si>
+  <si>
+    <t>e3S</t>
+  </si>
+  <si>
+    <t>D1D</t>
+  </si>
+  <si>
+    <t>E1P</t>
+  </si>
+  <si>
+    <t>f3D</t>
+  </si>
+  <si>
+    <t>F1S</t>
+  </si>
+  <si>
+    <t>G1P</t>
+  </si>
+  <si>
+    <t>H1S</t>
+  </si>
+  <si>
+    <t>g3S</t>
+  </si>
+  <si>
+    <t>h3P</t>
+  </si>
+  <si>
+    <t>i3S</t>
+  </si>
+  <si>
+    <t>I1S</t>
+  </si>
+  <si>
+    <t>j3P</t>
+  </si>
+  <si>
+    <t>J1P</t>
+  </si>
+  <si>
+    <t>K1D</t>
+  </si>
+  <si>
+    <t>k3D</t>
+  </si>
+  <si>
+    <t>L1S</t>
+  </si>
+  <si>
+    <t>l3S</t>
+  </si>
+  <si>
+    <t>M1P</t>
+  </si>
+  <si>
+    <t>m3P</t>
+  </si>
+  <si>
+    <t>n3P</t>
+  </si>
+  <si>
+    <t>o3S</t>
+  </si>
+  <si>
+    <t>N1D</t>
+  </si>
+  <si>
+    <t>O1S</t>
+  </si>
+  <si>
+    <t>P1S</t>
+  </si>
+  <si>
+    <t>p3D</t>
+  </si>
+  <si>
+    <t>Q1P</t>
+  </si>
+  <si>
+    <t>q3S</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>X1S</t>
+  </si>
+  <si>
+    <t>a3S</t>
+  </si>
+  <si>
+    <t>b3P</t>
+  </si>
+  <si>
+    <t>A1S</t>
+  </si>
+  <si>
+    <t>c3S</t>
+  </si>
+  <si>
+    <t>B1P</t>
+  </si>
+  <si>
+    <t>d3P</t>
+  </si>
+  <si>
+    <t>C1S</t>
+  </si>
+  <si>
+    <t>e3S</t>
+  </si>
+  <si>
+    <t>D1D</t>
+  </si>
+  <si>
+    <t>E1P</t>
+  </si>
+  <si>
+    <t>f3D</t>
+  </si>
+  <si>
+    <t>F1S</t>
+  </si>
+  <si>
+    <t>G1P</t>
+  </si>
+  <si>
+    <t>H1S</t>
+  </si>
+  <si>
+    <t>g3S</t>
+  </si>
+  <si>
+    <t>h3P</t>
+  </si>
+  <si>
+    <t>i3S</t>
+  </si>
+  <si>
+    <t>I1S</t>
+  </si>
+  <si>
+    <t>j3P</t>
+  </si>
+  <si>
+    <t>J1P</t>
+  </si>
+  <si>
+    <t>K1D</t>
+  </si>
+  <si>
+    <t>k3D</t>
+  </si>
+  <si>
+    <t>L1S</t>
+  </si>
+  <si>
+    <t>l3S</t>
+  </si>
+  <si>
+    <t>M1P</t>
+  </si>
+  <si>
+    <t>m3P</t>
+  </si>
+  <si>
+    <t>n3P</t>
+  </si>
+  <si>
+    <t>o3S</t>
+  </si>
+  <si>
+    <t>N1D</t>
+  </si>
+  <si>
+    <t>O1S</t>
+  </si>
+  <si>
+    <t>P1S</t>
+  </si>
+  <si>
+    <t>p3D</t>
+  </si>
+  <si>
+    <t>Q1P</t>
+  </si>
+  <si>
+    <t>q3S</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>X1S</t>
+  </si>
+  <si>
+    <t>a3S</t>
+  </si>
+  <si>
+    <t>b3P</t>
+  </si>
+  <si>
+    <t>A1S</t>
+  </si>
+  <si>
+    <t>c3S</t>
+  </si>
+  <si>
+    <t>B1P</t>
+  </si>
+  <si>
+    <t>d3P</t>
+  </si>
+  <si>
+    <t>C1S</t>
+  </si>
+  <si>
+    <t>e3S</t>
+  </si>
+  <si>
+    <t>D1D</t>
+  </si>
+  <si>
+    <t>E1P</t>
+  </si>
+  <si>
+    <t>f3D</t>
+  </si>
+  <si>
+    <t>F1S</t>
+  </si>
+  <si>
+    <t>G1P</t>
+  </si>
+  <si>
+    <t>H1S</t>
+  </si>
+  <si>
+    <t>g3S</t>
+  </si>
+  <si>
+    <t>h3P</t>
+  </si>
+  <si>
+    <t>i3S</t>
+  </si>
+  <si>
+    <t>I1S</t>
+  </si>
+  <si>
+    <t>j3P</t>
+  </si>
+  <si>
+    <t>J1P</t>
+  </si>
+  <si>
+    <t>K1D</t>
+  </si>
+  <si>
+    <t>k3D</t>
+  </si>
+  <si>
+    <t>L1S</t>
+  </si>
+  <si>
+    <t>l3S</t>
+  </si>
+  <si>
+    <t>M1P</t>
+  </si>
+  <si>
+    <t>m3P</t>
+  </si>
+  <si>
+    <t>n3P</t>
+  </si>
+  <si>
+    <t>o3S</t>
+  </si>
+  <si>
+    <t>N1D</t>
+  </si>
+  <si>
+    <t>O1S</t>
+  </si>
+  <si>
+    <t>P1S</t>
+  </si>
+  <si>
+    <t>p3D</t>
+  </si>
+  <si>
+    <t>Q1P</t>
+  </si>
+  <si>
+    <t>q3S</t>
+  </si>
   <si>
     <t>R</t>
   </si>
@@ -141,7 +465,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -150,13 +474,19 @@
       <diagonal/>
     </border>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -170,151 +500,151 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="true"/>
-    <col min="2" max="2" width="9.42578125" customWidth="true"/>
-    <col min="3" max="3" width="9.42578125" customWidth="true"/>
-    <col min="4" max="4" width="9.42578125" customWidth="true"/>
-    <col min="5" max="5" width="9.42578125" customWidth="true"/>
-    <col min="6" max="6" width="9.42578125" customWidth="true"/>
-    <col min="7" max="7" width="10.42578125" customWidth="true"/>
-    <col min="8" max="8" width="9.42578125" customWidth="true"/>
-    <col min="9" max="9" width="9.42578125" customWidth="true"/>
-    <col min="10" max="10" width="9.42578125" customWidth="true"/>
-    <col min="11" max="11" width="9.42578125" customWidth="true"/>
-    <col min="12" max="12" width="9.42578125" customWidth="true"/>
-    <col min="13" max="13" width="9.42578125" customWidth="true"/>
-    <col min="14" max="14" width="9.42578125" customWidth="true"/>
-    <col min="15" max="15" width="9.42578125" customWidth="true"/>
-    <col min="16" max="16" width="9.42578125" customWidth="true"/>
-    <col min="17" max="17" width="9.42578125" customWidth="true"/>
-    <col min="18" max="18" width="9.42578125" customWidth="true"/>
-    <col min="19" max="19" width="9.42578125" customWidth="true"/>
-    <col min="20" max="20" width="9.42578125" customWidth="true"/>
-    <col min="21" max="21" width="9.42578125" customWidth="true"/>
-    <col min="22" max="22" width="9.42578125" customWidth="true"/>
-    <col min="23" max="23" width="9.42578125" customWidth="true"/>
-    <col min="24" max="24" width="9.42578125" customWidth="true"/>
-    <col min="25" max="25" width="9.42578125" customWidth="true"/>
-    <col min="26" max="26" width="9.42578125" customWidth="true"/>
-    <col min="27" max="27" width="10.42578125" customWidth="true"/>
-    <col min="28" max="28" width="9.42578125" customWidth="true"/>
-    <col min="29" max="29" width="9.42578125" customWidth="true"/>
-    <col min="30" max="30" width="9.42578125" customWidth="true"/>
-    <col min="31" max="31" width="9.42578125" customWidth="true"/>
-    <col min="32" max="32" width="9.42578125" customWidth="true"/>
-    <col min="33" max="33" width="9.42578125" customWidth="true"/>
-    <col min="34" max="34" width="9.42578125" customWidth="true"/>
-    <col min="35" max="35" width="10.42578125" customWidth="true"/>
-    <col min="36" max="36" width="9.42578125" customWidth="true"/>
+    <col min="2" max="2" width="9.37890625" customWidth="true"/>
+    <col min="3" max="3" width="9.37890625" customWidth="true"/>
+    <col min="4" max="4" width="9.37890625" customWidth="true"/>
+    <col min="5" max="5" width="9.37890625" customWidth="true"/>
+    <col min="6" max="6" width="9.37890625" customWidth="true"/>
+    <col min="7" max="7" width="10.37890625" customWidth="true"/>
+    <col min="8" max="8" width="9.37890625" customWidth="true"/>
+    <col min="9" max="9" width="9.37890625" customWidth="true"/>
+    <col min="10" max="10" width="9.37890625" customWidth="true"/>
+    <col min="11" max="11" width="9.37890625" customWidth="true"/>
+    <col min="12" max="12" width="9.37890625" customWidth="true"/>
+    <col min="13" max="13" width="9.37890625" customWidth="true"/>
+    <col min="14" max="14" width="9.37890625" customWidth="true"/>
+    <col min="15" max="15" width="9.37890625" customWidth="true"/>
+    <col min="16" max="16" width="9.37890625" customWidth="true"/>
+    <col min="17" max="17" width="9.37890625" customWidth="true"/>
+    <col min="18" max="18" width="9.37890625" customWidth="true"/>
+    <col min="19" max="19" width="9.37890625" customWidth="true"/>
+    <col min="20" max="20" width="9.37890625" customWidth="true"/>
+    <col min="21" max="21" width="9.37890625" customWidth="true"/>
+    <col min="22" max="22" width="9.37890625" customWidth="true"/>
+    <col min="23" max="23" width="9.37890625" customWidth="true"/>
+    <col min="24" max="24" width="9.37890625" customWidth="true"/>
+    <col min="25" max="25" width="9.37890625" customWidth="true"/>
+    <col min="26" max="26" width="9.37890625" customWidth="true"/>
+    <col min="27" max="27" width="10.37890625" customWidth="true"/>
+    <col min="28" max="28" width="9.37890625" customWidth="true"/>
+    <col min="29" max="29" width="9.37890625" customWidth="true"/>
+    <col min="30" max="30" width="9.37890625" customWidth="true"/>
+    <col min="31" max="31" width="9.37890625" customWidth="true"/>
+    <col min="32" max="32" width="9.37890625" customWidth="true"/>
+    <col min="33" max="33" width="9.37890625" customWidth="true"/>
+    <col min="34" max="34" width="9.37890625" customWidth="true"/>
+    <col min="35" max="35" width="10.37890625" customWidth="true"/>
+    <col min="36" max="36" width="9.37890625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>110</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>7</v>
+        <v>115</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>11</v>
+        <v>119</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>15</v>
+        <v>123</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>16</v>
+        <v>124</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>18</v>
+        <v>126</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>19</v>
+        <v>127</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>20</v>
+        <v>128</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>22</v>
+        <v>130</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>23</v>
+        <v>131</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>24</v>
+        <v>132</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>25</v>
+        <v>133</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>26</v>
+        <v>134</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>27</v>
+        <v>135</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>29</v>
+        <v>137</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>31</v>
+        <v>139</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>32</v>
+        <v>140</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>35</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2">

</xml_diff>